<commit_message>
update state prior to converting schedule to use gt
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01600E21-17E0-644F-B712-7508C3496C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE26ADE-3905-1C4C-B859-9FEADA1576F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="7860" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="7620" yWindow="1760" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,10 +365,10 @@
     <t>00-reading.html</t>
   </si>
   <si>
-    <t>hw-01.html</t>
-  </si>
-  <si>
     <t>00-course-overview.html</t>
+  </si>
+  <si>
+    <t>hw-01</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,7 +786,7 @@
         <v>108</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F2" t="s">
         <v>104</v>
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
switched schedule to use gt()
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE26ADE-3905-1C4C-B859-9FEADA1576F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C914F26C-E568-EE49-B8D7-5CFFEA35F31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="1760" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="7600" yWindow="4540" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -347,9 +347,6 @@
     <t>Fri, Nov 18</t>
   </si>
   <si>
-    <t>Mon, Dec 16 2pm-5pm (usual classroom)</t>
-  </si>
-  <si>
     <t>lab-00-getting-started.html</t>
   </si>
   <si>
@@ -369,6 +366,9 @@
   </si>
   <si>
     <t>hw-01</t>
+  </si>
+  <si>
+    <t>Sat, Dec 16 2pm-5pm (in classroom)</t>
   </si>
 </sst>
 </file>
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -766,10 +766,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -783,13 +783,13 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" t="s">
         <v>108</v>
       </c>
-      <c r="E2" t="s">
-        <v>109</v>
-      </c>
       <c r="F2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -801,7 +801,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -824,7 +824,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
@@ -1198,7 +1198,7 @@
         <v>85</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add schedule with pdf links
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F161AA8F-6AB6-9043-A45D-574D939B7583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13420234-0814-1347-9861-55BBBF5F8367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7600" yWindow="3660" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
   <si>
     <t>Week</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>hw-11</t>
+  </si>
+  <si>
+    <t>16-bma/16-bma.pdf</t>
   </si>
 </sst>
 </file>
@@ -793,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1147,6 +1150,9 @@
       <c r="C29" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="E29" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="G29" t="s">
         <v>122</v>
       </c>

</xml_diff>

<commit_message>
add pdf for slide link
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BE2C56-B196-6A4C-957D-D7EE41E63AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5252403-0359-964B-9477-3CFEB9E2A0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="3660" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="7800" yWindow="6300" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -269,9 +269,6 @@
     <t>00-reading.html</t>
   </si>
   <si>
-    <t>00-course-overview.html</t>
-  </si>
-  <si>
     <t>hw-01</t>
   </si>
   <si>
@@ -423,6 +420,9 @@
   </si>
   <si>
     <t>lab-01-r-review.html</t>
+  </si>
+  <si>
+    <t>00-course-overview</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -848,7 +848,7 @@
         <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>128</v>
       </c>
       <c r="F2" t="s">
         <v>72</v>
@@ -875,7 +875,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18">
@@ -889,10 +889,10 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18">
@@ -904,7 +904,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
@@ -927,10 +927,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18">
@@ -942,7 +942,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18">
@@ -965,10 +965,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18">
@@ -980,7 +980,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18">
@@ -997,22 +997,22 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>23</v>
@@ -1021,7 +1021,7 @@
     <row r="16" spans="1:7" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -1032,19 +1032,19 @@
         <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>27</v>
@@ -1053,7 +1053,7 @@
     <row r="19" spans="1:7" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>31</v>
@@ -1064,7 +1064,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>33</v>
@@ -1073,7 +1073,7 @@
     <row r="21" spans="1:7" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>34</v>
@@ -1082,7 +1082,7 @@
     <row r="22" spans="1:7" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>30</v>
@@ -1093,7 +1093,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>29</v>
@@ -1102,19 +1102,19 @@
     <row r="24" spans="1:7" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18">
@@ -1122,7 +1122,7 @@
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>36</v>
@@ -1131,7 +1131,7 @@
     <row r="27" spans="1:7" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>37</v>
@@ -1140,7 +1140,7 @@
     <row r="28" spans="1:7" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>38</v>
@@ -1151,22 +1151,22 @@
         <v>39</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>41</v>
@@ -1175,7 +1175,7 @@
     <row r="31" spans="1:7" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>42</v>
@@ -1186,19 +1186,19 @@
         <v>43</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>45</v>
@@ -1207,7 +1207,7 @@
     <row r="34" spans="1:7" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>46</v>
@@ -1218,19 +1218,19 @@
         <v>47</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>49</v>
@@ -1239,7 +1239,7 @@
     <row r="37" spans="1:7" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>50</v>
@@ -1250,19 +1250,19 @@
         <v>47</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>52</v>
@@ -1273,19 +1273,19 @@
         <v>53</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>55</v>
@@ -1294,7 +1294,7 @@
     <row r="42" spans="1:7" ht="18">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>56</v>
@@ -1314,7 +1314,7 @@
         <v>59</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Lecture 1 to schedule (pdf & html)
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FF7413-CDC6-B94C-9C5A-3A0998BE6ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEF58FF-F786-2C4B-B3D3-2A553BFC2498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="3660" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="6580" yWindow="6560" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -425,7 +425,7 @@
     <t>00-course-overview</t>
   </si>
   <si>
-    <t>00-basics-of-bayes</t>
+    <t>01-basics-of-bayes</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
add html and figs for lecture 2
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEF58FF-F786-2C4B-B3D3-2A553BFC2498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A12989-43B2-8E4D-8ABC-74F3FB467243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="6560" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
   <si>
     <t>Week</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>01-basics-of-bayes</t>
+  </si>
+  <si>
+    <t>02-loss-functions</t>
   </si>
 </sst>
 </file>
@@ -803,7 +806,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -897,6 +900,9 @@
       <c r="D5" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="E5" t="s">
+        <v>130</v>
+      </c>
       <c r="G5" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Add lecture 3 slides
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A12989-43B2-8E4D-8ABC-74F3FB467243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4584F5F0-D700-7841-B37D-A8923E8BF004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="6560" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="132">
   <si>
     <t>Week</t>
   </si>
@@ -429,6 +429,9 @@
   </si>
   <si>
     <t>02-loss-functions</t>
+  </si>
+  <si>
+    <t>03-normal-predictive-distributions</t>
   </si>
 </sst>
 </file>
@@ -806,7 +809,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -918,6 +921,9 @@
       <c r="D6" s="2" t="s">
         <v>80</v>
       </c>
+      <c r="E6" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="7" spans="1:7" ht="18">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
add lab2 and start updating lecture 4
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4584F5F0-D700-7841-B37D-A8923E8BF004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78457B5C-8BF9-A346-BE8C-EC671D81699F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="133">
   <si>
     <t>Week</t>
   </si>
@@ -432,6 +432,9 @@
   </si>
   <si>
     <t>03-normal-predictive-distributions</t>
+  </si>
+  <si>
+    <t>lab-02-beta-binomial.html</t>
   </si>
 </sst>
 </file>
@@ -809,7 +812,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -933,6 +936,9 @@
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="F7" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="18">
       <c r="A8" s="2" t="s">

</xml_diff>

<commit_message>
add updated lecture 4
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78457B5C-8BF9-A346-BE8C-EC671D81699F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B3CB0-06A0-C94B-85A2-D304AA19E6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="134">
   <si>
     <t>Week</t>
   </si>
@@ -435,6 +435,9 @@
   </si>
   <si>
     <t>lab-02-beta-binomial.html</t>
+  </si>
+  <si>
+    <t>04-predictive-checks</t>
   </si>
 </sst>
 </file>
@@ -812,7 +815,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -953,6 +956,9 @@
       <c r="D8" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="E8" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="G8" s="2" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
fix typos in slides fix links to readings
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7B3CB0-06A0-C94B-85A2-D304AA19E6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4627CB3-F734-A74E-A969-0720664C760E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -281,21 +281,9 @@
     <t>03-reading.html</t>
   </si>
   <si>
-    <t>04-readings.html</t>
-  </si>
-  <si>
-    <t>05-readings.html</t>
-  </si>
-  <si>
-    <t>06-readings.html</t>
-  </si>
-  <si>
     <t>07-readings.html</t>
   </si>
   <si>
-    <t>08-readings.html</t>
-  </si>
-  <si>
     <t>Tues, Sept 26</t>
   </si>
   <si>
@@ -438,6 +426,18 @@
   </si>
   <si>
     <t>04-predictive-checks</t>
+  </si>
+  <si>
+    <t>04-reading.html</t>
+  </si>
+  <si>
+    <t>05-reading.html</t>
+  </si>
+  <si>
+    <t>06-reading.html</t>
+  </si>
+  <si>
+    <t>08-reading.html</t>
   </si>
 </sst>
 </file>
@@ -815,7 +815,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -863,7 +863,7 @@
         <v>76</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s">
         <v>72</v>
@@ -881,7 +881,7 @@
         <v>75</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18">
@@ -893,7 +893,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18">
@@ -910,7 +910,7 @@
         <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G5" t="s">
         <v>77</v>
@@ -928,7 +928,7 @@
         <v>80</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
@@ -940,7 +940,7 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18">
@@ -954,13 +954,13 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18">
@@ -972,7 +972,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18">
@@ -995,10 +995,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18">
@@ -1010,7 +1010,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18">
@@ -1027,22 +1027,22 @@
         <v>21</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>23</v>
@@ -1051,7 +1051,7 @@
     <row r="16" spans="1:7" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
@@ -1062,19 +1062,19 @@
         <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>27</v>
@@ -1083,7 +1083,7 @@
     <row r="19" spans="1:7" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>31</v>
@@ -1094,7 +1094,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>33</v>
@@ -1103,7 +1103,7 @@
     <row r="21" spans="1:7" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>34</v>
@@ -1112,7 +1112,7 @@
     <row r="22" spans="1:7" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>30</v>
@@ -1123,7 +1123,7 @@
         <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>29</v>
@@ -1132,19 +1132,19 @@
     <row r="24" spans="1:7" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G24" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18">
@@ -1152,7 +1152,7 @@
         <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>36</v>
@@ -1161,7 +1161,7 @@
     <row r="27" spans="1:7" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>37</v>
@@ -1170,7 +1170,7 @@
     <row r="28" spans="1:7" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>38</v>
@@ -1181,22 +1181,22 @@
         <v>39</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G29" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>41</v>
@@ -1205,7 +1205,7 @@
     <row r="31" spans="1:7" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>42</v>
@@ -1216,19 +1216,19 @@
         <v>43</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>44</v>
       </c>
       <c r="G32" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>45</v>
@@ -1237,7 +1237,7 @@
     <row r="34" spans="1:7" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>46</v>
@@ -1248,19 +1248,19 @@
         <v>47</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G35" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>49</v>
@@ -1269,7 +1269,7 @@
     <row r="37" spans="1:7" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>50</v>
@@ -1280,19 +1280,19 @@
         <v>47</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>51</v>
       </c>
       <c r="G38" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>52</v>
@@ -1303,19 +1303,19 @@
         <v>53</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>54</v>
       </c>
       <c r="G40" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>55</v>
@@ -1324,7 +1324,7 @@
     <row r="42" spans="1:7" ht="18">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
add lab3 link to github classsroom
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA21D01-C7BD-C043-8D68-98F728F63796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244506D5-4689-554C-BA19-C687FFF8E536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="136">
   <si>
     <t>Week</t>
   </si>
@@ -441,6 +441,9 @@
   </si>
   <si>
     <t>05-hierarchical-models</t>
+  </si>
+  <si>
+    <t>lab-03.html</t>
   </si>
 </sst>
 </file>
@@ -818,7 +821,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -989,6 +992,9 @@
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F10" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="18">
       <c r="A11" s="2" t="s">

</xml_diff>

<commit_message>
add lecture 6: metropolis
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{244506D5-4689-554C-BA19-C687FFF8E536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38B415F-6504-B94A-AAC7-8E3E21BC4147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="137">
   <si>
     <t>Week</t>
   </si>
@@ -444,6 +444,9 @@
   </si>
   <si>
     <t>lab-03.html</t>
+  </si>
+  <si>
+    <t>06-metropolis</t>
   </si>
 </sst>
 </file>
@@ -821,7 +824,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1009,6 +1012,9 @@
       <c r="D11" s="2" t="s">
         <v>132</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="G11" s="2" t="s">
         <v>112</v>
       </c>

</xml_diff>

<commit_message>
add lecture 7 and readings
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBD929F-7D5E-8A4B-9D29-32463B3E0084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D17326-4B4B-AB4D-8AF6-9B1F007A92C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="138">
   <si>
     <t>Week</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Lecture 6: Metropolis Algorithm &amp; Stochastic Sampling</t>
   </si>
   <si>
-    <t>Lecture 7: More MCMC - Metropolis Hastings and Adaptive Metropolis</t>
-  </si>
-  <si>
     <t>Lab 4: Metropolis Hastings</t>
   </si>
   <si>
@@ -447,6 +444,12 @@
   </si>
   <si>
     <t>06-metropolis</t>
+  </si>
+  <si>
+    <t>07-adaptive-metropolis</t>
+  </si>
+  <si>
+    <t>Lecture 7: Diagnostics and Adaptive Metropolis</t>
   </si>
 </sst>
 </file>
@@ -824,7 +827,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -852,10 +855,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18">
@@ -863,46 +866,46 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18">
@@ -910,46 +913,46 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18">
@@ -957,46 +960,46 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18">
@@ -1004,365 +1007,368 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18">
       <c r="A14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18">
       <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="G17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18">
       <c r="A20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18">
       <c r="A26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18">
       <c r="A29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18">
       <c r="A32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18">
       <c r="A35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="G35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18">
       <c r="A38" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18">
       <c r="A40" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="G40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18">
       <c r="A43" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18">
       <c r="A44" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed typo for 07-reading link
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D17326-4B4B-AB4D-8AF6-9B1F007A92C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ADABE8-6F7A-604E-B551-B25A5ACFBC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="139">
   <si>
     <t>Week</t>
   </si>
@@ -278,9 +278,6 @@
     <t>03-reading.html</t>
   </si>
   <si>
-    <t>07-readings.html</t>
-  </si>
-  <si>
     <t>Tues, Sept 26</t>
   </si>
   <si>
@@ -450,6 +447,12 @@
   </si>
   <si>
     <t>Lecture 7: Diagnostics and Adaptive Metropolis</t>
+  </si>
+  <si>
+    <t>07-reading.html</t>
+  </si>
+  <si>
+    <t>09-reading.html</t>
   </si>
 </sst>
 </file>
@@ -827,7 +830,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -875,7 +878,7 @@
         <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F2" t="s">
         <v>71</v>
@@ -893,7 +896,7 @@
         <v>74</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18">
@@ -905,7 +908,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18">
@@ -922,7 +925,7 @@
         <v>78</v>
       </c>
       <c r="E5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G5" t="s">
         <v>76</v>
@@ -940,7 +943,7 @@
         <v>79</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
@@ -952,7 +955,7 @@
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18">
@@ -966,13 +969,13 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18">
@@ -984,10 +987,10 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18">
@@ -999,7 +1002,7 @@
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18">
@@ -1013,13 +1016,13 @@
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18">
@@ -1028,13 +1031,13 @@
         <v>70</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18">
@@ -1051,31 +1054,34 @@
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>23</v>
@@ -1086,19 +1092,19 @@
         <v>24</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>26</v>
@@ -1107,7 +1113,7 @@
     <row r="19" spans="1:7" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>30</v>
@@ -1118,7 +1124,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>32</v>
@@ -1127,7 +1133,7 @@
     <row r="21" spans="1:7" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>33</v>
@@ -1136,7 +1142,7 @@
     <row r="22" spans="1:7" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>29</v>
@@ -1147,7 +1153,7 @@
         <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>28</v>
@@ -1156,19 +1162,19 @@
     <row r="24" spans="1:7" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18">
@@ -1176,7 +1182,7 @@
         <v>34</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>35</v>
@@ -1185,7 +1191,7 @@
     <row r="27" spans="1:7" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>36</v>
@@ -1194,7 +1200,7 @@
     <row r="28" spans="1:7" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>37</v>
@@ -1205,22 +1211,22 @@
         <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>40</v>
@@ -1229,7 +1235,7 @@
     <row r="31" spans="1:7" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>41</v>
@@ -1240,19 +1246,19 @@
         <v>42</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>44</v>
@@ -1261,7 +1267,7 @@
     <row r="34" spans="1:7" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>45</v>
@@ -1272,19 +1278,19 @@
         <v>46</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>48</v>
@@ -1293,7 +1299,7 @@
     <row r="37" spans="1:7" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>49</v>
@@ -1304,19 +1310,19 @@
         <v>46</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>50</v>
       </c>
       <c r="G38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>51</v>
@@ -1327,19 +1333,19 @@
         <v>52</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>53</v>
       </c>
       <c r="G40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>54</v>
@@ -1348,7 +1354,7 @@
     <row r="42" spans="1:7" ht="18">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
add lab 4 to schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01ADABE8-6F7A-604E-B551-B25A5ACFBC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D77991-A852-8D4C-BFD9-98CA63BB829B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="140">
   <si>
     <t>Week</t>
   </si>
@@ -453,6 +453,9 @@
   </si>
   <si>
     <t>09-reading.html</t>
+  </si>
+  <si>
+    <t>lab-04.html</t>
   </si>
 </sst>
 </file>
@@ -830,7 +833,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1048,6 +1051,9 @@
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F13" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="18">
       <c r="A14" s="2" t="s">

</xml_diff>

<commit_message>
add lecture 8 html and qmd
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D77991-A852-8D4C-BFD9-98CA63BB829B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940B1739-30DC-244C-BAF5-7A385AF1F1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="141">
   <si>
     <t>Week</t>
   </si>
@@ -456,6 +456,9 @@
   </si>
   <si>
     <t>lab-04.html</t>
+  </si>
+  <si>
+    <t>08-gibbs</t>
   </si>
 </sst>
 </file>
@@ -833,7 +836,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1068,6 +1071,9 @@
       <c r="D14" s="2" t="s">
         <v>131</v>
       </c>
+      <c r="E14" s="2" t="s">
+        <v>140</v>
+      </c>
       <c r="G14" s="2" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
update to add lecture 9 DA and update schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940B1739-30DC-244C-BAF5-7A385AF1F1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E91CC8-0EC0-B647-AB2B-BFDBDD89C348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="146">
   <si>
     <t>Week</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Lecture 9: Data Augmentation</t>
   </si>
   <si>
-    <t>Lab 5: Adaptive Metropolis Hastings</t>
-  </si>
-  <si>
     <t>WEEK 6</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
     <t>NO CLASS FALL BREAK</t>
   </si>
   <si>
-    <t>Midterm I</t>
-  </si>
-  <si>
     <t>Lab 6: Hypothesis &amp; Multiple Testing</t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>Lec 17: Bayesian Variable Selection and Model Averaging</t>
   </si>
   <si>
-    <t>Lab: Q&amp;A with HW 7</t>
-  </si>
-  <si>
     <t>Week 11</t>
   </si>
   <si>
@@ -377,9 +368,6 @@
     <t>hw-05</t>
   </si>
   <si>
-    <t>Lab: Q &amp; A</t>
-  </si>
-  <si>
     <t>hw-06</t>
   </si>
   <si>
@@ -459,6 +447,33 @@
   </si>
   <si>
     <t>08-gibbs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab 5:  Gibbs, DA and Adaptive Metropolis </t>
+  </si>
+  <si>
+    <t>Lecture 10: Missing Data</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>Lec 18:</t>
+  </si>
+  <si>
+    <t>Lec 19:  Outliers</t>
+  </si>
+  <si>
+    <t>Midterm 1</t>
+  </si>
+  <si>
+    <t>Lab: Review</t>
+  </si>
+  <si>
+    <t>09-Data-augmentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab: Q&amp;A </t>
   </si>
 </sst>
 </file>
@@ -833,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -847,7 +862,7 @@
     <col min="6" max="6" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18">
+    <row r="1" spans="1:8" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -864,529 +879,568 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18">
+        <v>70</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="18">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="18">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="18">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="18">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="18">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="18">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="18">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="18">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="18">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="18">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="18">
+        <v>134</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18">
+      <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="18">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="18">
+    </row>
+    <row r="18" spans="1:8" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="18">
+        <v>25</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="18">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="18">
-      <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="18">
+      <c r="G20" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="18">
+        <v>31</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="18">
+      <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="18">
-      <c r="A23" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="B23" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="18">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="18">
+        <v>87</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="18">
+        <v>35</v>
+      </c>
+      <c r="G25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="18">
       <c r="A26" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="18">
+        <v>33</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="18">
+        <v>34</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="18">
+      <c r="A29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="18">
-      <c r="A29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="18">
+        <v>116</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18">
+        <v>38</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="18">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>43</v>
+        <v>140</v>
       </c>
       <c r="G32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="18">
+        <v>112</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="18">
+        <v>141</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="18">
+      <c r="A35" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="18">
-      <c r="A35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="C35" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="18">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="18">
+      <c r="A38" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="18">
-      <c r="A38" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G38" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="18">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="18">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="18">
       <c r="A40" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G40" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="18">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="18">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="18">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="18">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="18">
       <c r="A43" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="18">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="18">
       <c r="A44" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update readings for lecture 9 & 10, plus schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E91CC8-0EC0-B647-AB2B-BFDBDD89C348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18751D30-B02F-CE48-A0F0-8AADD388F0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="148">
   <si>
     <t>Week</t>
   </si>
@@ -474,6 +474,12 @@
   </si>
   <si>
     <t xml:space="preserve">Lab: Q&amp;A </t>
+  </si>
+  <si>
+    <t>10-reading.html</t>
+  </si>
+  <si>
+    <t>10-missing-data</t>
   </si>
 </sst>
 </file>
@@ -850,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1130,6 +1136,12 @@
       <c r="C17" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="D17" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="G17" t="s">
         <v>109</v>
       </c>

</xml_diff>

<commit_message>
fix typo in schedule and broken link
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18751D30-B02F-CE48-A0F0-8AADD388F0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080102FB-1C6E-9D47-93AD-B3388A012A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -470,9 +470,6 @@
     <t>Lab: Review</t>
   </si>
   <si>
-    <t>09-Data-augmentation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lab: Q&amp;A </t>
   </si>
   <si>
@@ -480,6 +477,9 @@
   </si>
   <si>
     <t>10-missing-data</t>
+  </si>
+  <si>
+    <t>09-data-augmentation</t>
   </si>
 </sst>
 </file>
@@ -857,7 +857,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1114,7 +1114,7 @@
         <v>134</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
@@ -1137,10 +1137,10 @@
         <v>138</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="G17" t="s">
         <v>109</v>
@@ -1310,7 +1310,7 @@
         <v>94</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18">

</xml_diff>

<commit_message>
update to include link to lab5
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080102FB-1C6E-9D47-93AD-B3388A012A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0A4C4D-328B-F94E-98EF-36D841A210D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="150">
   <si>
     <t>Week</t>
   </si>
@@ -122,9 +122,6 @@
     <t>NO CLASS FALL BREAK</t>
   </si>
   <si>
-    <t>Lab 6: Hypothesis &amp; Multiple Testing</t>
-  </si>
-  <si>
     <t>WEEK 8</t>
   </si>
   <si>
@@ -480,6 +477,15 @@
   </si>
   <si>
     <t>09-data-augmentation</t>
+  </si>
+  <si>
+    <t>lab-05.html</t>
+  </si>
+  <si>
+    <t>Lecture 11: Bayes Linear Regression and Priors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab 6: </t>
   </si>
 </sst>
 </file>
@@ -857,7 +863,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -885,13 +891,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18">
@@ -899,46 +905,46 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18">
@@ -946,46 +952,46 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18">
@@ -993,46 +999,46 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18">
@@ -1040,46 +1046,46 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18">
@@ -1087,43 +1093,46 @@
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="F16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18">
@@ -1131,19 +1140,19 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="G17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>24</v>
@@ -1152,10 +1161,10 @@
     <row r="18" spans="1:8" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>25</v>
@@ -1164,10 +1173,10 @@
     <row r="19" spans="1:8" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18">
@@ -1175,45 +1184,45 @@
         <v>26</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>27</v>
@@ -1222,237 +1231,237 @@
     <row r="24" spans="1:8" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18">
       <c r="A26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="H26" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18">
       <c r="A29" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18">
       <c r="A32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G32" t="s">
+        <v>111</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G32" t="s">
-        <v>112</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18">
       <c r="A35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18">
       <c r="A38" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18">
       <c r="A40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="G40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18">
       <c r="A43" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18">
       <c r="A44" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add lecture 11 on Bayes regressions
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78731B7-B334-6842-9291-C3B373A43E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17D982C-2455-934E-ADAF-9F517330F66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="3640" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="10060" yWindow="4320" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="153">
   <si>
     <t>Week</t>
   </si>
@@ -486,6 +486,15 @@
   </si>
   <si>
     <t xml:space="preserve">Lab 6: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lab 7: </t>
+  </si>
+  <si>
+    <t>11-reading.html</t>
+  </si>
+  <si>
+    <t>11-bayes-regression</t>
   </si>
 </sst>
 </file>
@@ -863,7 +872,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1166,6 +1175,12 @@
       <c r="C18" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="D18" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>152</v>
+      </c>
       <c r="H18" s="2" t="s">
         <v>25</v>
       </c>
@@ -1243,10 +1258,13 @@
         <v>87</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="G25" t="s">
         <v>110</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18">

</xml_diff>

<commit_message>
current draft of lecture 12
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAF454F-ABD5-514E-BF5A-A2F504DA6CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7E6410-76E0-A04A-9E85-7F91696E8565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="4320" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="7800" yWindow="3540" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="158">
   <si>
     <t>Week</t>
   </si>
@@ -485,9 +485,6 @@
     <t>Lecture 11: Bayes Linear Regression and Priors</t>
   </si>
   <si>
-    <t xml:space="preserve">Lab 6: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Lab 7: </t>
   </si>
   <si>
@@ -495,6 +492,24 @@
   </si>
   <si>
     <t>11-bayes-regression</t>
+  </si>
+  <si>
+    <t>Lab 6:  Q &amp; A on HW 5 &amp; Missing Data</t>
+  </si>
+  <si>
+    <t>Lec 14:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lec 15: </t>
+  </si>
+  <si>
+    <t>Lec 12: Choice of Priors in  Regression</t>
+  </si>
+  <si>
+    <t>12-reading.html</t>
+  </si>
+  <si>
+    <t>12-priors-regressions</t>
   </si>
 </sst>
 </file>
@@ -872,7 +887,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1176,10 +1191,10 @@
         <v>148</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>25</v>
@@ -1191,7 +1206,7 @@
         <v>81</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18">
@@ -1202,7 +1217,13 @@
         <v>82</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>29</v>
+        <v>155</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="G20" t="s">
         <v>109</v>
@@ -1258,7 +1279,7 @@
         <v>87</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G25" t="s">
         <v>110</v>
@@ -1275,7 +1296,7 @@
         <v>88</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>32</v>
@@ -1287,7 +1308,7 @@
         <v>89</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>154</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
add pdf and fix typo in schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7E6410-76E0-A04A-9E85-7F91696E8565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26423225-9CE2-504E-8AC5-50E7B130B8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7800" yWindow="3540" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="158">
   <si>
     <t>Week</t>
   </si>
@@ -128,15 +128,9 @@
     <t>Lec 12: Multiple Testing and Hierachical Models</t>
   </si>
   <si>
-    <t>Lec 13: Bayesian Multiple Testing and Hierachical Models</t>
-  </si>
-  <si>
     <t>WEEK 9</t>
   </si>
   <si>
-    <t>Lec 14: Bayesian Linear Regression</t>
-  </si>
-  <si>
     <t>Lec 15: Priors in Bayesian Linear Regression</t>
   </si>
   <si>
@@ -497,19 +491,25 @@
     <t>Lab 6:  Q &amp; A on HW 5 &amp; Missing Data</t>
   </si>
   <si>
-    <t>Lec 14:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lec 15: </t>
-  </si>
-  <si>
     <t>Lec 12: Choice of Priors in  Regression</t>
   </si>
   <si>
     <t>12-reading.html</t>
   </si>
   <si>
-    <t>12-priors-regressions</t>
+    <t>12-priors-regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lec 13: </t>
+  </si>
+  <si>
+    <t>Lec 15:  Bayesian Multiple Testing and Hierachical Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lec 14: </t>
+  </si>
+  <si>
+    <t>Lec 13:  Mixtures of Conjugate Priors</t>
   </si>
 </sst>
 </file>
@@ -887,7 +887,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -915,13 +915,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18">
@@ -929,46 +929,46 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18">
@@ -976,46 +976,46 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18">
@@ -1023,46 +1023,46 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18">
@@ -1070,46 +1070,46 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18">
@@ -1117,46 +1117,46 @@
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18">
@@ -1164,19 +1164,19 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>24</v>
@@ -1185,16 +1185,16 @@
     <row r="18" spans="1:8" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>25</v>
@@ -1203,10 +1203,10 @@
     <row r="19" spans="1:8" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18">
@@ -1214,19 +1214,19 @@
         <v>26</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>29</v>
@@ -1235,22 +1235,22 @@
     <row r="21" spans="1:8" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>30</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
@@ -1258,7 +1258,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>27</v>
@@ -1267,240 +1267,238 @@
     <row r="24" spans="1:8" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18">
       <c r="A29" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18">
       <c r="A32" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18">
       <c r="A35" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18">
       <c r="A38" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G38" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18">
       <c r="A40" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18">
       <c r="A43" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18">
       <c r="A44" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add review materials for lab
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D4A254-64BD-D143-94A5-12469EE77766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63B0625-5C40-C643-B952-7021BD91C61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="3540" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="6340" yWindow="3720" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="162">
   <si>
     <t>Week</t>
   </si>
@@ -458,9 +458,6 @@
     <t>Midterm 1</t>
   </si>
   <si>
-    <t>Lab: Review</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lab: Q&amp;A </t>
   </si>
   <si>
@@ -479,9 +476,6 @@
     <t>Lecture 11: Bayes Linear Regression and Priors</t>
   </si>
   <si>
-    <t xml:space="preserve">Lab 7: </t>
-  </si>
-  <si>
     <t>11-reading.html</t>
   </si>
   <si>
@@ -516,6 +510,18 @@
   </si>
   <si>
     <t>13-reading.html</t>
+  </si>
+  <si>
+    <t>Lab 7: Dimension Reduction via Regularization</t>
+  </si>
+  <si>
+    <t>Lab 6: Dimension Reduction via Regularization</t>
+  </si>
+  <si>
+    <t>lab-midterm-I-review.html</t>
+  </si>
+  <si>
+    <t>Lab : Review for Midterm I</t>
   </si>
 </sst>
 </file>
@@ -893,7 +899,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1150,7 +1156,7 @@
         <v>131</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
@@ -1162,7 +1168,7 @@
         <v>134</v>
       </c>
       <c r="F16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18">
@@ -1176,10 +1182,10 @@
         <v>135</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="G17" t="s">
         <v>106</v>
@@ -1194,13 +1200,13 @@
         <v>78</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>25</v>
@@ -1212,7 +1218,7 @@
         <v>79</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18">
@@ -1223,13 +1229,13 @@
         <v>80</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>29</v>
@@ -1241,19 +1247,19 @@
         <v>81</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G21" t="s">
         <v>107</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18">
@@ -1262,7 +1268,10 @@
         <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>140</v>
+        <v>161</v>
+      </c>
+      <c r="F22" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
@@ -1291,13 +1300,10 @@
         <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G25" t="s">
-        <v>108</v>
+        <v>159</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18">
@@ -1308,7 +1314,10 @@
         <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
+      </c>
+      <c r="G26" t="s">
+        <v>108</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -1318,7 +1327,7 @@
         <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>31</v>
@@ -1368,7 +1377,7 @@
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18">

</xml_diff>

<commit_message>
add lab6 to the schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FFC901-FD76-374A-99CC-A97E251BBE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81012EC-05C6-1041-A4D2-4616BA6952D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="4420" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="7800" yWindow="3540" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="161">
   <si>
     <t>Week</t>
   </si>
@@ -506,9 +506,6 @@
     <t>13-reading.html</t>
   </si>
   <si>
-    <t>Lab 6: Dimension Reduction via Regularization</t>
-  </si>
-  <si>
     <t>lab-midterm-I-review.html</t>
   </si>
   <si>
@@ -516,6 +513,12 @@
   </si>
   <si>
     <t>Lec 14:  Basics of Bayesian Hypothesis Tests</t>
+  </si>
+  <si>
+    <t>Lab 6: Shrinkage Priors in Regression Comparison</t>
+  </si>
+  <si>
+    <t>lab-06.html</t>
   </si>
 </sst>
 </file>
@@ -893,7 +896,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1260,10 +1263,10 @@
         <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
@@ -1292,7 +1295,10 @@
         <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
+      </c>
+      <c r="F25" t="s">
+        <v>160</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -1304,7 +1310,7 @@
         <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G26" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
initial draft of Lecture 14 & readings
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D44A04-D922-BF42-A2C2-DF534669CADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14DF488-8622-C54E-A9A0-7E6B36750160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="3540" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="2340" yWindow="6260" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="163">
   <si>
     <t>Week</t>
   </si>
@@ -519,6 +519,12 @@
   </si>
   <si>
     <t>Lecture 11: Bayes Linear Regression</t>
+  </si>
+  <si>
+    <t>14-hypothesis-testing</t>
+  </si>
+  <si>
+    <t>14-reading.html</t>
   </si>
 </sst>
 </file>
@@ -895,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1312,6 +1318,12 @@
       <c r="C26" s="2" t="s">
         <v>157</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" t="s">
+        <v>161</v>
+      </c>
       <c r="G26" t="s">
         <v>108</v>
       </c>

</xml_diff>

<commit_message>
add HW7 and draft lecture 15
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14DF488-8622-C54E-A9A0-7E6B36750160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36115A14-8632-BC4E-8CEF-9D98E97FA518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="6260" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="160">
   <si>
     <t>Week</t>
   </si>
@@ -110,12 +110,6 @@
     <t>WEEK 6</t>
   </si>
   <si>
-    <t>Lecture 10: Basics of Hypothesis Testing</t>
-  </si>
-  <si>
-    <t>Lecture 11: Hypothesis Testing</t>
-  </si>
-  <si>
     <t>WEEK 7</t>
   </si>
   <si>
@@ -125,18 +119,12 @@
     <t>WEEK 8</t>
   </si>
   <si>
-    <t>Lec 12: Multiple Testing and Hierachical Models</t>
-  </si>
-  <si>
     <t>WEEK 9</t>
   </si>
   <si>
     <t>Lec 15: Priors in Bayesian Linear Regression</t>
   </si>
   <si>
-    <t>Lab 7: Variable Selection</t>
-  </si>
-  <si>
     <t>WEEK 10</t>
   </si>
   <si>
@@ -152,9 +140,6 @@
     <t>Lec 18: Outliers</t>
   </si>
   <si>
-    <t>Lec 19: Missing Data</t>
-  </si>
-  <si>
     <t>Lab 8: Review</t>
   </si>
   <si>
@@ -525,6 +510,12 @@
   </si>
   <si>
     <t>14-reading.html</t>
+  </si>
+  <si>
+    <t>15-reading.html</t>
+  </si>
+  <si>
+    <t>Lab 7:  Multiple Hypothesis Testing</t>
   </si>
 </sst>
 </file>
@@ -901,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="93" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -930,13 +921,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18">
@@ -944,46 +935,46 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18">
@@ -991,46 +982,46 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18">
@@ -1038,46 +1029,46 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18">
@@ -1085,46 +1076,46 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18">
@@ -1132,46 +1123,46 @@
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F16" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18">
@@ -1179,355 +1170,350 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G21" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F22" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F25" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="18">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="E26" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G26" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
+      </c>
+      <c r="D27" t="s">
+        <v>158</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>32</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18">
       <c r="A32" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G32" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G35" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G38" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18">
       <c r="A40" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G40" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18">
       <c r="A43" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18">
       <c r="A44" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upload lab & HW 8, update schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3008E10C-DF03-144E-B961-F988FED624A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC15B0BB-31AF-5540-A78D-294C11F9E1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8120" yWindow="1380" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="4640" yWindow="5200" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="162">
   <si>
     <t>Week</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Lec 18: Outliers</t>
   </si>
   <si>
-    <t>Lab 8: Review</t>
-  </si>
-  <si>
     <t>Week 12</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>Lec 20: Random Effects</t>
   </si>
   <si>
-    <t>Lab 9</t>
-  </si>
-  <si>
     <t>Lec 21: Mixed Effects Models</t>
   </si>
   <si>
@@ -428,18 +422,9 @@
     <t>Old</t>
   </si>
   <si>
-    <t>Lec 18:</t>
-  </si>
-  <si>
-    <t>Lec 19:  Outliers</t>
-  </si>
-  <si>
     <t>Midterm 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Lab: Q&amp;A </t>
-  </si>
-  <si>
     <t>10-reading.html</t>
   </si>
   <si>
@@ -522,6 +507,21 @@
   </si>
   <si>
     <t>16-bma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lec 19: </t>
+  </si>
+  <si>
+    <t>Lab 8: Variable Selection</t>
+  </si>
+  <si>
+    <t>lab-08.html</t>
+  </si>
+  <si>
+    <t>Lab 9: Review</t>
+  </si>
+  <si>
+    <t>Lab 11</t>
   </si>
 </sst>
 </file>
@@ -898,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="93" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -927,13 +927,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18">
@@ -941,46 +941,46 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18">
@@ -988,46 +988,46 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18">
@@ -1035,46 +1035,46 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18">
@@ -1082,46 +1082,46 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18">
@@ -1129,46 +1129,46 @@
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F16" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18">
@@ -1176,45 +1176,45 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18">
@@ -1222,48 +1222,48 @@
         <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="G21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F22" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
@@ -1271,7 +1271,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>25</v>
@@ -1280,22 +1280,22 @@
     <row r="24" spans="1:8" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F25" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -1304,48 +1304,48 @@
         <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="E26" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D27" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F28" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18">
@@ -1353,43 +1353,42 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>30</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>133</v>
+        <v>158</v>
+      </c>
+      <c r="F31" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18">
@@ -1397,136 +1396,133 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H32" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>131</v>
+        <v>157</v>
+      </c>
+      <c r="G33" t="s">
+        <v>102</v>
       </c>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>33</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18">
       <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G35" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="G36" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18">
       <c r="A38" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="G39" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G40" t="s">
-        <v>106</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18">
       <c r="A43" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18">
       <c r="A44" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix typo and add readings
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F6C94C-FA1A-0A4C-8816-BBFB453701D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B760C8D6-9D00-794A-844F-5A755993E682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4640" yWindow="3580" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="166">
   <si>
     <t>Week</t>
   </si>
@@ -528,6 +528,12 @@
   </si>
   <si>
     <t>Lec 19:  Random Effects</t>
+  </si>
+  <si>
+    <t>18-reading.html</t>
+  </si>
+  <si>
+    <t>17-reading.html</t>
   </si>
 </sst>
 </file>
@@ -905,7 +911,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="93" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1380,6 +1386,9 @@
       <c r="C30" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="D30" t="s">
+        <v>165</v>
+      </c>
       <c r="E30" t="s">
         <v>161</v>
       </c>
@@ -1410,6 +1419,9 @@
       <c r="C32" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="D32" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="E32" s="2" t="s">
         <v>162</v>
       </c>

</xml_diff>

<commit_message>
add readings for Thursday
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B760C8D6-9D00-794A-844F-5A755993E682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CCCA3E-423F-8A4E-9FAB-5DB222FFEA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4640" yWindow="3580" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="168">
   <si>
     <t>Week</t>
   </si>
@@ -534,6 +534,12 @@
   </si>
   <si>
     <t>17-reading.html</t>
+  </si>
+  <si>
+    <t>19-reading.html</t>
+  </si>
+  <si>
+    <t>19-random-effects</t>
   </si>
 </sst>
 </file>
@@ -911,7 +917,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1434,6 +1440,12 @@
       <c r="C33" s="2" t="s">
         <v>163</v>
       </c>
+      <c r="D33" t="s">
+        <v>166</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="G33" t="s">
         <v>102</v>
       </c>

</xml_diff>

<commit_message>
Add midterm review to schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CCCA3E-423F-8A4E-9FAB-5DB222FFEA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB52DEE-21E5-4442-855C-C29EDF08DD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4640" yWindow="3580" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="169">
   <si>
     <t>Week</t>
   </si>
@@ -540,6 +540,9 @@
   </si>
   <si>
     <t>19-random-effects</t>
+  </si>
+  <si>
+    <t>lab-midterm-II-review.html</t>
   </si>
 </sst>
 </file>
@@ -917,7 +920,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="93" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1459,6 +1462,9 @@
       <c r="C34" s="2" t="s">
         <v>159</v>
       </c>
+      <c r="F34" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="18">
       <c r="A35" s="2" t="s">

</xml_diff>

<commit_message>
Add lecture on mixed effects and readings
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6967857A-AE47-D847-8944-53FFEB33A35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850D9027-C535-DB48-97BB-97550855C34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="3580" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="11380" yWindow="6700" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="172">
   <si>
     <t>Week</t>
   </si>
@@ -143,12 +143,6 @@
     <t>Midterm II</t>
   </si>
   <si>
-    <t>Lec 20: Random Effects</t>
-  </si>
-  <si>
-    <t>Lec 21: Mixed Effects Models</t>
-  </si>
-  <si>
     <t>Thanksgiving Break - No Class </t>
   </si>
   <si>
@@ -161,9 +155,6 @@
     <t>BARK: NonParametric Regression</t>
   </si>
   <si>
-    <t>Lab 10</t>
-  </si>
-  <si>
     <t>Week 14</t>
   </si>
   <si>
@@ -543,6 +534,24 @@
   </si>
   <si>
     <t>lab-midterm-II-review.html</t>
+  </si>
+  <si>
+    <t>Lec 20: Mixed Effects Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lec 21: Hamiltonian Monte Carlo </t>
+  </si>
+  <si>
+    <t>lab-10.html</t>
+  </si>
+  <si>
+    <t>20-mixed-effects</t>
+  </si>
+  <si>
+    <t>Lab 10:  Random Effect Models in stan</t>
+  </si>
+  <si>
+    <t>20-reading.html</t>
   </si>
 </sst>
 </file>
@@ -919,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="93" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="93" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -948,13 +957,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18">
@@ -962,46 +971,46 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18">
@@ -1009,46 +1018,46 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="18">
@@ -1056,46 +1065,46 @@
         <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18">
@@ -1103,46 +1112,46 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="18">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="18">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="18">
@@ -1150,46 +1159,46 @@
         <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="18">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18">
@@ -1197,45 +1206,45 @@
         <v>23</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="E17" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="18">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18">
@@ -1243,48 +1252,48 @@
         <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="18">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="18">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18">
@@ -1292,7 +1301,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>25</v>
@@ -1301,22 +1310,22 @@
     <row r="24" spans="1:8" ht="18">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F25" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -1325,48 +1334,48 @@
         <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E26" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G26" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="18">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="18">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F28" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18">
@@ -1374,48 +1383,48 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" ht="18">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E30" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" ht="18">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F31" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18">
@@ -1423,47 +1432,47 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" t="s">
         <v>163</v>
       </c>
-      <c r="D33" t="s">
-        <v>166</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G33" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" ht="18">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F34" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18">
@@ -1471,7 +1480,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>34</v>
@@ -1480,22 +1489,31 @@
     <row r="36" spans="1:8" ht="18">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>35</v>
+        <v>166</v>
+      </c>
+      <c r="D36" t="s">
+        <v>171</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="G36" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>41</v>
+        <v>170</v>
+      </c>
+      <c r="F37" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18">
@@ -1503,68 +1521,68 @@
         <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>36</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G39" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18">
       <c r="A40" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="18">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="18">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="18">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="18">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add old finals for review
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A54CF95-C68C-EC45-9603-64012C26C43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC41CE0-3A10-AB48-B51E-2A190316DF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="3740" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
+    <workbookView xWindow="7800" yWindow="3540" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="179">
   <si>
     <t>Week</t>
   </si>
@@ -570,6 +570,9 @@
   </si>
   <si>
     <t>23-BARK</t>
+  </si>
+  <si>
+    <t>final-review.html</t>
   </si>
 </sst>
 </file>
@@ -946,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225F965B-3C0C-EF4C-8875-E04C1032D9DF}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="93" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1623,6 +1626,9 @@
       <c r="B44" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="D44" t="s">
+        <v>178</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix schedule for final review
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clyde/Documents/Github/STA702-F23/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC41CE0-3A10-AB48-B51E-2A190316DF3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27EBEFC-D423-5E41-84C1-A003C8EADD81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7800" yWindow="3540" windowWidth="28040" windowHeight="17440" xr2:uid="{E4FBF6DA-300C-7541-B141-2AEBAADFFCB9}"/>
   </bookViews>
@@ -950,7 +950,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="93" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1626,7 +1626,7 @@
       <c r="B44" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D44" t="s">
+      <c r="F44" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>